<commit_message>
Added core test classes
</commit_message>
<xml_diff>
--- a/NALBDDCucSel/TestData-FW/TestData.xlsx
+++ b/NALBDDCucSel/TestData-FW/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8638b6d2aa5a54b9/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohd Yusuf\codeRepository\NALCucSelBDD\NALBDDCucSel\TestData-FW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67550697-CF37-4FC1-9BBA-EBE0FCF1B0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E47D79E-5B2E-4F15-A304-0911A3E5E994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40F0057E-5E72-49FF-99C3-6D6D67539A93}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{40F0057E-5E72-49FF-99C3-6D6D67539A93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>yusuf</t>
+  </si>
+  <si>
+    <t>Khan</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C7E738-E384-408F-B31A-D210EAE84742}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,6 +435,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>